<commit_message>
Correct size for better print
</commit_message>
<xml_diff>
--- a/Checklist Datos2.xlsx
+++ b/Checklist Datos2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\OMIXOM\Datos2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC29507-5F89-4CDB-B1AF-5EDA8F7A6616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094FBEF4-2C45-49D0-AACE-116AA19E65B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED264797-A6AF-4AE6-8175-48CD6CF14227}"/>
   </bookViews>
@@ -443,10 +443,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -555,25 +555,6 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -617,13 +598,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -641,6 +615,32 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -656,11 +656,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F4E82FB-C45E-4FED-BE9C-30A1E9AC8C4F}" name="Table1" displayName="Table1" ref="B1:G22" totalsRowShown="0" headerRowDxfId="4" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F4E82FB-C45E-4FED-BE9C-30A1E9AC8C4F}" name="Table1" displayName="Table1" ref="B1:G22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B1:G22" xr:uid="{5F4E82FB-C45E-4FED-BE9C-30A1E9AC8C4F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{24DE67DE-9887-45C7-A086-51BD5F9A45CE}" name="Impresiones" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{471D14AA-6A86-4CBE-82AC-9661D380F813}" name="Tengo" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{24DE67DE-9887-45C7-A086-51BD5F9A45CE}" name="Impresiones" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{471D14AA-6A86-4CBE-82AC-9661D380F813}" name="Tengo" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{C1E5E144-39A1-45BF-8446-C105FEBFE9E9}" name="Electronica" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{57A7C7D3-255F-4B8E-87E9-3BBEC0A49ACC}" name="Tengo " dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{6270E6FB-A4CD-4460-9763-A9B12F123A77}" name="Ferreteria" dataDxfId="1"/>
@@ -990,12 +990,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
@@ -1026,7 +1026,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1043,7 +1043,7 @@
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1073,7 +1073,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>52</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
@@ -1118,7 +1118,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1165,7 +1165,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="2" t="s">
         <v>55</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1225,7 +1225,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>58</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1272,7 +1272,7 @@
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="2" t="s">
         <v>61</v>
       </c>
@@ -1302,7 +1302,7 @@
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1319,7 +1319,7 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>64</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="6" t="s">
         <v>66</v>
       </c>
@@ -1356,7 +1356,7 @@
     <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Add dupont terminal row
</commit_message>
<xml_diff>
--- a/Checklist Datos2.xlsx
+++ b/Checklist Datos2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio\Documents\OMIXOM\Datos2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC86395-D770-4E12-9572-86BA12EC865C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABFC420-C032-47F1-AB21-421C3CFF6251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED264797-A6AF-4AE6-8175-48CD6CF14227}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Impresiones</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>Terminales Dupont</t>
   </si>
 </sst>
 </file>
@@ -993,7 +996,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1284,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
@@ -1296,7 +1299,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
@@ -1313,7 +1316,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
@@ -1328,7 +1331,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
@@ -1342,8 +1345,8 @@
         <v>66</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
-        <v>67</v>
+      <c r="D22" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">

</xml_diff>